<commit_message>
Cambios generales, interfaz de salud añadida, enemigo con salud añadida, 3 ataques básicos añadidos
</commit_message>
<xml_diff>
--- a/animaciones_pendientes.xlsx
+++ b/animaciones_pendientes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Animaciones pendientes</t>
   </si>
@@ -146,16 +146,31 @@
   <si>
     <t>Salto hacia Atras</t>
   </si>
+  <si>
+    <t>Ataque aereo</t>
+  </si>
+  <si>
+    <t>Ataque agachado</t>
+  </si>
+  <si>
+    <t>Knockback Debil</t>
+  </si>
+  <si>
+    <t>Knockback Medio</t>
+  </si>
+  <si>
+    <t>Knockback Fuerte</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -190,7 +205,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -198,14 +213,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,18 +249,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -273,16 +296,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,7 +312,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -305,14 +320,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,6 +329,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,13 +381,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,7 +441,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,97 +531,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,55 +555,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -579,30 +594,21 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -627,7 +633,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,16 +662,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -677,152 +692,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -845,62 +860,59 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
+    <cellStyle name="Coma" xfId="6" builtinId="3"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21"/>
+    <cellStyle name="Nota" xfId="11" builtinId="10"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
+    <cellStyle name="Título" xfId="14" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
+    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
+    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
+    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
+    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
+    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
+    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
+    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
+    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -943,8 +955,28 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" val="0"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" val="0"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2828,6 +2860,636 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="5350510" y="4716780"/>
+              <a:ext cx="913765" cy="205740"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr wrap="square" anchor="ctr" upright="1">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="es-MX"/>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:ea typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:cs typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:sym typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>225425</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>17780</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>468630</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>223520</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5350510" y="4970780"/>
+              <a:ext cx="913765" cy="205740"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr wrap="square" anchor="ctr" upright="1">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="es-MX"/>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:ea typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:cs typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:sym typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>225425</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>17780</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>468630</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>223520</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1043"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5350510" y="5199380"/>
+              <a:ext cx="913765" cy="205740"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr wrap="square" anchor="ctr" upright="1">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="es-MX"/>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:ea typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:cs typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:sym typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>225425</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>17780</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>468630</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>223520</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1044"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5350510" y="5466080"/>
+              <a:ext cx="913765" cy="205740"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr wrap="square" anchor="ctr" upright="1">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="es-MX"/>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:ea typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:cs typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:sym typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>225425</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>17780</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>468630</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>223520</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1045"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5350510" y="5707380"/>
+              <a:ext cx="913765" cy="205740"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr wrap="square" anchor="ctr" upright="1">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle>
+              <a:defPPr>
+                <a:defRPr lang="es-MX"/>
+              </a:defPPr>
+              <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl1pPr>
+              <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl2pPr>
+              <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl3pPr>
+              <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl4pPr>
+              <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl5pPr>
+              <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl6pPr>
+              <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl7pPr>
+              <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl8pPr>
+              <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+                <a:defRPr sz="1100">
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:lvl9pPr>
+            </a:lstStyle>
+            <a:p>
+              <a:pPr algn="l" rtl="0"/>
+              <a:endParaRPr lang="zh-CN" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:ea typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:cs typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+                <a:sym typeface="Tahoma" panose="020B0604030504040204" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>225425</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>17780</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>468630</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>33020</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1046"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5350510" y="5948680"/>
               <a:ext cx="913765" cy="205740"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3186,10 +3848,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:E21"/>
+  <dimension ref="C3:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -3350,8 +4012,50 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="8"/>
+    <row r="21" ht="18" customHeight="1" spans="3:5">
+      <c r="C21" s="3">
+        <v>17</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" ht="21" customHeight="1" spans="3:5">
+      <c r="C22" s="3">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" ht="19" customHeight="1" spans="3:5">
+      <c r="C23" s="3">
+        <v>19</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" ht="19" customHeight="1" spans="3:5">
+      <c r="C24" s="3">
+        <v>20</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="3:5">
+      <c r="C25" s="3">
+        <v>21</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3716,6 +4420,116 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1042" name="Check Box 18" r:id="rId19">
+              <controlPr defaultSize="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>225425</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>17780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>468630</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>223520</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1043" name="Check Box 19" r:id="rId20">
+              <controlPr defaultSize="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>225425</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>17780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>468630</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>223520</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1044" name="Check Box 20" r:id="rId21">
+              <controlPr defaultSize="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>225425</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>17780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>468630</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>223520</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1045" name="Check Box 21" r:id="rId22">
+              <controlPr defaultSize="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>225425</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>17780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>468630</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>223520</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1046" name="Check Box 22" r:id="rId23">
+              <controlPr defaultSize="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>225425</xdr:colOff>
+                    <xdr:row>24</xdr:row>
+                    <xdr:rowOff>17780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>468630</xdr:colOff>
+                    <xdr:row>25</xdr:row>
+                    <xdr:rowOff>33020</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>

<commit_message>
Mecanica de arma y apuntado lista, leves mejoras en los ataques, ataque aereo añadido, ahora las balas son RigidBody en lugar de KinematicBody
</commit_message>
<xml_diff>
--- a/animaciones_pendientes.xlsx
+++ b/animaciones_pendientes.xlsx
@@ -14,18 +14,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Animaciones pendientes</t>
+  </si>
+  <si>
+    <t>Tipos de knockback</t>
+  </si>
+  <si>
+    <t>funcion damaged(arg1, arg2, arg3)</t>
   </si>
   <si>
     <t>Quieto</t>
   </si>
   <si>
+    <t>weak_damage</t>
+  </si>
+  <si>
+    <t>damageRecieved</t>
+  </si>
+  <si>
+    <t>Daño que recibe la entidad</t>
+  </si>
+  <si>
     <t>Correr</t>
   </si>
   <si>
+    <t>medium_damage</t>
+  </si>
+  <si>
+    <t>knockbackPower</t>
+  </si>
+  <si>
+    <t>Valor del empuje que recibe</t>
+  </si>
+  <si>
     <t>Agacharse</t>
+  </si>
+  <si>
+    <t>heavy_damage</t>
+  </si>
+  <si>
+    <t>knockbackType</t>
+  </si>
+  <si>
+    <t>Tipo de knockback</t>
   </si>
   <si>
     <t>Caminar Agachado</t>
@@ -75,6 +108,9 @@
       </rPr>
       <t xml:space="preserve"> con Arma</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <r>
@@ -205,7 +241,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -220,14 +256,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -258,6 +317,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -266,23 +333,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,6 +347,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -312,23 +364,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -342,13 +378,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,13 +417,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,13 +459,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,67 +549,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,61 +567,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +609,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,6 +648,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -614,17 +677,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,15 +693,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -679,11 +729,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -692,13 +740,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -713,131 +761,131 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -861,6 +909,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3848,59 +3911,107 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:E25"/>
+  <dimension ref="C3:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="49.4380952380952" customWidth="1"/>
     <col min="5" max="5" width="10.0571428571429" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="35.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" ht="11" customHeight="1"/>
-    <row r="4" ht="29" customHeight="1" spans="3:5">
+    <row r="4" ht="29" customHeight="1" spans="3:15">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
+      <c r="I4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="M4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
     </row>
-    <row r="5" ht="20" customHeight="1" spans="3:5">
+    <row r="5" ht="20" customHeight="1" spans="3:15">
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5"/>
+      <c r="I5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="M5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" ht="20" customHeight="1" spans="3:5">
+    <row r="6" ht="20" customHeight="1" spans="3:15">
       <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5"/>
+      <c r="I6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="M6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" ht="20" customHeight="1" spans="3:5">
+    <row r="7" ht="20" customHeight="1" spans="3:15">
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E7" s="5"/>
+      <c r="I7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="M7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1" spans="3:5">
       <c r="C8" s="3">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5"/>
     </row>
@@ -3909,25 +4020,28 @@
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" ht="20" customHeight="1" spans="3:5">
+    <row r="10" ht="20" customHeight="1" spans="3:16">
       <c r="C10" s="3">
         <v>6</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5"/>
+      <c r="P10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1" spans="3:5">
       <c r="C11" s="3">
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -3936,7 +4050,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -3945,7 +4059,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -3954,7 +4068,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -3963,7 +4077,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E15" s="5"/>
     </row>
@@ -3972,7 +4086,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E16" s="5"/>
     </row>
@@ -3981,7 +4095,7 @@
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E17" s="5"/>
     </row>
@@ -3990,7 +4104,7 @@
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E18" s="5"/>
     </row>
@@ -3999,7 +4113,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E19" s="5"/>
     </row>
@@ -4008,7 +4122,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E20" s="5"/>
     </row>
@@ -4017,7 +4131,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E21" s="5"/>
     </row>
@@ -4026,7 +4140,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E22" s="5"/>
     </row>
@@ -4035,7 +4149,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E23" s="5"/>
     </row>
@@ -4044,7 +4158,7 @@
         <v>20</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E24" s="5"/>
     </row>
@@ -4053,13 +4167,21 @@
         <v>21</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E25" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="9">
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="M7:N7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>